<commit_message>
Se agrego los nuevos campos de tipomaderable y unidad de medida en especies aprobadas del plan general
</commit_message>
<xml_diff>
--- a/SIGOFCv3/Archivos/Plantilla/EspeciesAprobadas.xlsx
+++ b/SIGOFCv3/Archivos/Plantilla/EspeciesAprobadas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021-Proyectos\Osinfor_F02_015\SIGOFCv3\Archivos\Plantilla\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CONDOR\repos\SIGOsfc\SIGOFCv3\Archivos\Plantilla\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C79483C-EF7A-4A44-9CC6-99560CE6FE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Datos" sheetId="1" r:id="rId1"/>
@@ -918,7 +917,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1899">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3094" uniqueCount="1907">
   <si>
     <t>NOMBRE_CIENTIFICO</t>
   </si>
@@ -6615,12 +6614,36 @@
   </si>
   <si>
     <t>Bloque N° 8</t>
+  </si>
+  <si>
+    <t>TIPOMADERABLE</t>
+  </si>
+  <si>
+    <t>UNIDAD_MEDIDA</t>
+  </si>
+  <si>
+    <t>CARBON</t>
+  </si>
+  <si>
+    <t>MADERABLES</t>
+  </si>
+  <si>
+    <t>NO MADERABLES</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>LT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -6770,13 +6793,13 @@
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal 4" xfId="5" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Normal 5" xfId="3" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Normal 6" xfId="4" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Normal 7" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Normal 8" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 4" xfId="5"/>
+    <cellStyle name="Normal 5" xfId="3"/>
+    <cellStyle name="Normal 6" xfId="4"/>
+    <cellStyle name="Normal 7" xfId="6"/>
+    <cellStyle name="Normal 8" xfId="7"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -6867,23 +6890,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -6919,23 +6925,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -7111,12 +7100,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7129,7 +7118,7 @@
     <col min="6" max="16384" width="20.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7144,33 +7133,51 @@
       </c>
       <c r="E1" s="1" t="s">
         <v>1892</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1899</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1900</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
       <formula1>INDIRECT(SUBSTITUTE(A12," ","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A1048576">
       <formula1>nombre_cientifico</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11 B16:B1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B11 B16:B1048576">
       <formula1>INDIRECT(SUBSTITUTE(A2," ","_"))</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" errorTitle="Error" error="Seleccione valor de la lista" sqref="D2:E915" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Seleccione valor de la lista" sqref="C1" xr:uid="{2DA27B62-D7B8-4ECD-9F2B-A71FBD873947}"/>
+    <dataValidation allowBlank="1" errorTitle="Error" error="Seleccione valor de la lista" sqref="D2:E915"/>
+    <dataValidation allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Seleccione valor de la lista" sqref="C1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Seleccione valor de la lista" xr:uid="{A4A15BB5-8D94-415D-9905-75C89145CE37}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Error" error="Seleccione valor de la lista">
           <x14:formula1>
             <xm:f>Hoja1!$A$1:$A$8</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja1!$C$1:$C$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Hoja1!$E$1:$E$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -7179,7 +7186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:AHK524"/>
   <sheetViews>
@@ -18179,7 +18186,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" columnSort="1" ref="A1:ABB10">
+  <sortState columnSort="1" ref="A1:ABB10">
     <sortCondition ref="A2:ABB2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18188,52 +18195,70 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja3"/>
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1889</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>1901</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1904</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1890</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>1902</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1893</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>1903</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1906</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1894</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>1895</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1896</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>1897</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1898</v>
       </c>
@@ -18241,5 +18266,6 @@
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>